<commit_message>
reran all processing steps with newly cleaned data
</commit_message>
<xml_diff>
--- a/experiments/2021_car_inner_clock_bhi/results/statistics/stats_imu_features_condition.xlsx
+++ b/experiments/2021_car_inner_clock_bhi/results/statistics/stats_imu_features_condition.xlsx
@@ -50,19 +50,19 @@
     <t>normal</t>
   </si>
   <si>
-    <t>ss_max_60</t>
-  </si>
-  <si>
-    <t>ss_max_position</t>
-  </si>
-  <si>
-    <t>ss_mean_60</t>
-  </si>
-  <si>
-    <t>ss_number_60</t>
-  </si>
-  <si>
-    <t>ss_std_60</t>
+    <t>sm_max_60</t>
+  </si>
+  <si>
+    <t>sm_max_position</t>
+  </si>
+  <si>
+    <t>sm_mean_60</t>
+  </si>
+  <si>
+    <t>sm_number_60</t>
+  </si>
+  <si>
+    <t>sm_std_60</t>
   </si>
   <si>
     <t>Known Alarm</t>

</xml_diff>